<commit_message>
changed according to payload structure
</commit_message>
<xml_diff>
--- a/utilities/pgr_dataLoader/upload/Tenant_Master.xlsx
+++ b/utilities/pgr_dataLoader/upload/Tenant_Master.xlsx
@@ -126,14 +126,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00C6EFCE"/>
-        <bgColor rgb="00C6EFCE"/>
+        <fgColor rgb="00FFEB9C"/>
+        <bgColor rgb="00FFEB9C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFEB9C"/>
-        <bgColor rgb="00FFEB9C"/>
+        <fgColor rgb="00C6EFCE"/>
+        <bgColor rgb="00C6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -157,7 +157,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
@@ -196,6 +196,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -3769,13 +3770,13 @@
   <dimension ref="A1:S1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col width="26.5" customWidth="1" min="1" max="1"/>
-    <col width="38.83203125" customWidth="1" min="2" max="2"/>
+    <col width="23" customWidth="1" min="2" max="2"/>
     <col width="25.5" customWidth="1" min="3" max="3"/>
     <col width="28.33203125" customWidth="1" min="4" max="4"/>
     <col width="15.5" customWidth="1" min="5" max="5"/>
@@ -3847,17 +3848,17 @@
       <c r="N1" s="8" t="n"/>
       <c r="O1" s="8" t="n"/>
       <c r="P1" s="8" t="n"/>
-      <c r="Q1" s="16" t="inlineStr">
+      <c r="Q1" s="17" t="inlineStr">
         <is>
           <t>_STATUS</t>
         </is>
       </c>
-      <c r="R1" s="16" t="inlineStr">
+      <c r="R1" s="17" t="inlineStr">
         <is>
           <t>_STATUS_CODE</t>
         </is>
       </c>
-      <c r="S1" s="16" t="inlineStr">
+      <c r="S1" s="17" t="inlineStr">
         <is>
           <t>_ERROR_MESSAGE</t>
         </is>
@@ -3866,48 +3867,48 @@
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="9" t="inlineStr">
         <is>
-          <t>City A ULB</t>
+          <t>State A</t>
         </is>
       </c>
       <c r="B2" s="9" t="inlineStr">
         <is>
-          <t>PG.CITYA</t>
+          <t>STATEA</t>
         </is>
       </c>
       <c r="C2" s="9" t="inlineStr">
         <is>
-          <t>City</t>
+          <t>State</t>
         </is>
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>./iamge</t>
+          <t>./sal</t>
         </is>
       </c>
       <c r="E2" s="8" t="n">
-        <v>32.4</v>
+        <v>49.34</v>
       </c>
       <c r="F2" s="8" t="n">
-        <v>43.44</v>
+        <v>59.43</v>
       </c>
       <c r="G2" s="9" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="H2" s="9" t="inlineStr">
+        <is>
+          <t>Karanataka</t>
+        </is>
+      </c>
+      <c r="I2" s="8" t="inlineStr">
         <is>
           <t>bangalore</t>
         </is>
       </c>
-      <c r="H2" s="9" t="inlineStr">
-        <is>
-          <t>adjkaks</t>
-        </is>
-      </c>
-      <c r="I2" s="8" t="inlineStr">
-        <is>
-          <t>dsadsa</t>
-        </is>
-      </c>
       <c r="J2" s="15" t="inlineStr">
         <is>
-          <t>https://localhost</t>
+          <t>https://karnataka.gov.in/english</t>
         </is>
       </c>
       <c r="K2" s="8" t="n"/>
@@ -3933,48 +3934,48 @@
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="10" t="inlineStr">
         <is>
-          <t>City</t>
+          <t>State citya</t>
         </is>
       </c>
-      <c r="B3" s="10" t="inlineStr">
+      <c r="B3" s="9" t="inlineStr">
         <is>
-          <t>PG</t>
+          <t>STATEA.CITY</t>
         </is>
       </c>
       <c r="C3" s="10" t="inlineStr">
         <is>
-          <t>State</t>
+          <t>City</t>
         </is>
       </c>
-      <c r="D3" s="8" t="inlineStr">
+      <c r="D3" s="11" t="inlineStr">
         <is>
-          <t>./iamge</t>
+          <t>.das</t>
         </is>
       </c>
-      <c r="E3" s="8" t="n">
-        <v>32.4</v>
+      <c r="E3" s="11" t="n">
+        <v>59.23</v>
       </c>
-      <c r="F3" s="8" t="n">
-        <v>43.44</v>
+      <c r="F3" s="11" t="n">
+        <v>43.55</v>
       </c>
       <c r="G3" s="9" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="H3" s="9" t="inlineStr">
+        <is>
+          <t>Karanataka</t>
+        </is>
+      </c>
+      <c r="I3" s="8" t="inlineStr">
         <is>
           <t>bangalore</t>
         </is>
       </c>
-      <c r="H3" s="9" t="inlineStr">
-        <is>
-          <t>adjkaks</t>
-        </is>
-      </c>
-      <c r="I3" s="8" t="inlineStr">
-        <is>
-          <t>dsadsa</t>
-        </is>
-      </c>
       <c r="J3" s="15" t="inlineStr">
         <is>
-          <t>https://localhost</t>
+          <t>https://karnataka.gov.in/english</t>
         </is>
       </c>
       <c r="K3" s="11" t="n"/>
@@ -21969,7 +21970,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -22004,56 +22005,52 @@
           <t>State Logo</t>
         </is>
       </c>
-      <c r="E1" s="16" t="inlineStr">
+      <c r="E1" s="17" t="inlineStr">
         <is>
           <t>_STATUS</t>
         </is>
       </c>
-      <c r="F1" s="16" t="inlineStr">
+      <c r="F1" s="17" t="inlineStr">
         <is>
           <t>_STATUS_CODE</t>
         </is>
       </c>
-      <c r="G1" s="16" t="inlineStr">
+      <c r="G1" s="17" t="inlineStr">
         <is>
           <t>_ERROR_MESSAGE</t>
         </is>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="13" t="inlineStr">
+      <c r="A2" s="16" t="inlineStr">
         <is>
-          <t>sadsa</t>
+          <t>https://karnataka.gov.in/english</t>
         </is>
       </c>
-      <c r="B2" s="13" t="inlineStr">
+      <c r="B2" s="16" t="inlineStr">
         <is>
-          <t>dsad</t>
+          <t>https://karnataka.gov.in/english</t>
         </is>
       </c>
-      <c r="C2" s="13" t="inlineStr">
+      <c r="C2" s="16" t="inlineStr">
         <is>
-          <t>dsada</t>
+          <t>https://karnataka.gov.in/english</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="16" t="inlineStr">
         <is>
-          <t>dsda</t>
+          <t>https://karnataka.gov.in/english</t>
         </is>
       </c>
-      <c r="E2" s="18" t="inlineStr">
+      <c r="E2" s="19" t="inlineStr">
         <is>
-          <t>EXISTS</t>
+          <t>SUCCESS</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>400</v>
+        <v>202</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>{"ResponseInfo":null,"Errors":[{"id":null,"parentId":null,"code":"DUPLICATE_RECORD","message":"Duplicate record","description":null,"params":null}]}</t>
-        </is>
-      </c>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="13" t="n"/>
@@ -28049,6 +28046,12 @@
       <formula1>REGEXMATCH(A2,"^(https?://).+")</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B2" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C2" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D2" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>